<commit_message>
Updated sync belt wheel
including the solidworks model of the wheel and the updated version of the parts list.
</commit_message>
<xml_diff>
--- a/Parts/零部件列表.xlsx
+++ b/Parts/零部件列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/yfdu_ucdavis_edu/Documents/FTC/2018个人项目/3D printer/Parts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="354" documentId="11_F25DC773A252ABDACC1048AD711B75305ADE58EB" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DE42F798-F82F-464D-BF2D-19D838E6DE50}"/>
+  <xr:revisionPtr revIDLastSave="402" documentId="11_F25DC773A252ABDACC1048AD711B75305ADE58EB" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3287969F-7F4A-40C2-B0AC-7A8964F11052}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
   <si>
     <t>结构分类</t>
   </si>
@@ -119,12 +119,6 @@
     <t>同步轮</t>
   </si>
   <si>
-    <t>2GT</t>
-  </si>
-  <si>
-    <t>内径6mm</t>
-  </si>
-  <si>
     <t>内径8mm</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t>模型名称</t>
   </si>
   <si>
-    <t>外径6mm</t>
-  </si>
-  <si>
     <t>外径8mm</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>https://item.taobao.com/item.htm?spm=a1z0k.7385961.1997985097.d4918997.741347faeyAEo8&amp;id=554589658438&amp;_u=t2dmg8j26111</t>
   </si>
   <si>
-    <t>330mm</t>
-  </si>
-  <si>
     <t>光轴固定架</t>
   </si>
   <si>
@@ -260,9 +248,6 @@
     <t>https://item.taobao.com/item.htm?spm=a1z10.5-c-s.w4002-16890816583.24.e97326cbXnisSV&amp;id=16409826759</t>
   </si>
   <si>
-    <t>2020 aluminum part</t>
-  </si>
-  <si>
     <t>2020 L-shaped connector plate</t>
   </si>
   <si>
@@ -335,13 +320,67 @@
     <t>8mm copper slide sleeve</t>
   </si>
   <si>
-    <t>6mm copper slide sleeve</t>
-  </si>
-  <si>
     <t>center slider</t>
   </si>
   <si>
     <t>侧横柱360mm</t>
+  </si>
+  <si>
+    <t>340mm</t>
+  </si>
+  <si>
+    <t>侧柱500-550mm</t>
+  </si>
+  <si>
+    <t>中心滑块</t>
+  </si>
+  <si>
+    <t>8mm copper slide sleeve 40mm</t>
+  </si>
+  <si>
+    <t>侧面滑块</t>
+  </si>
+  <si>
+    <t>2020 aluminum part 360mm</t>
+  </si>
+  <si>
+    <t>2020 aluminum part 500mm</t>
+  </si>
+  <si>
+    <t>8mm 20 teeth synchronous belt wheel (double belt compatible)</t>
+  </si>
+  <si>
+    <t>8mm 20 teeth synchronous belt wheel</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a1z0k.7386009.0.d4919233.6a0847fag2iqjv&amp;id=528360060257&amp;_u=t2dmg8j26111</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a1z0k.7386009.0.d4919233.6a0847fag2iqjv&amp;id=528687341718&amp;_u=t2dmg8j26111</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=2013.1.3.8.40f1b79fkkppxe&amp;id=527745858306</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=2013.1.3.6.1b8d4ceaVFkXV2&amp;id=527978862744</t>
+  </si>
+  <si>
+    <t>一卷1000mm</t>
+  </si>
+  <si>
+    <t>弹性联轴器</t>
+  </si>
+  <si>
+    <t>200mm</t>
+  </si>
+  <si>
+    <t>100mm</t>
+  </si>
+  <si>
+    <t>300mm</t>
+  </si>
+  <si>
+    <t>2GT/宽5mm</t>
   </si>
 </sst>
 </file>
@@ -386,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,10 +444,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -694,267 +739,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="1"/>
-    <col min="7" max="7" width="28.88671875" style="2" customWidth="1"/>
-    <col min="8" max="9" width="9.109375" style="1"/>
-    <col min="10" max="10" width="65.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="28.85546875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="65.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="10">
         <v>2020</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="H4" s="1">
         <v>6</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>53</v>
+      <c r="J4" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="K4" s="1">
         <f>H4*I4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="H5" s="1">
         <v>6</v>
       </c>
-      <c r="J5" s="9"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:K42" si="0">H5*I5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+        <f t="shared" ref="K5:K41" si="0">H5*I5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="H6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1">
         <v>2040</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="H7" s="1">
         <v>3</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="7">
+        <v>62</v>
+      </c>
+      <c r="C8" s="10">
         <v>2020</v>
       </c>
       <c r="H8" s="1">
         <v>4</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>62</v>
+        <v>69</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H9" s="3">
         <v>12</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
       <c r="G10" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H10" s="1">
         <v>40</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>71</v>
+      <c r="D11" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" s="7">
+        <v>72</v>
+      </c>
+      <c r="H11" s="10">
         <v>80</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="3"/>
       <c r="J12" s="5"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -962,179 +1016,182 @@
         <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="7"/>
+        <v>90</v>
+      </c>
+      <c r="H13" s="10"/>
       <c r="J13" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H14" s="1">
         <v>2</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>50</v>
+      <c r="J14" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H15" s="1">
         <v>4</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H16" s="1">
         <v>2</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="11"/>
       <c r="K16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H17" s="2">
         <v>4</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
       <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>39</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="9" t="s">
-        <v>65</v>
+      <c r="J18" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="K18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="11"/>
       <c r="K19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>29</v>
+      <c r="C20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>100</v>
@@ -1143,80 +1200,81 @@
         <v>2</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="1" t="s">
-        <v>30</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H21" s="1">
         <v>4</v>
       </c>
-      <c r="J21" s="9" t="s">
-        <v>58</v>
+      <c r="J21" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H22" s="1">
         <v>4</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="11"/>
       <c r="K22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1226,274 +1284,350 @@
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>63</v>
+        <v>44</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="H25" s="7">
+      <c r="H25" s="10">
         <v>8</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="J26" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="7"/>
-      <c r="J26" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="K26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="E29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="E30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="J30" s="11"/>
+      <c r="K30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="E31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32" s="1">
+        <v>10</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="10">
+        <v>42</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="K35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="K36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H27" s="7"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="K28" s="3">
-        <f>H28*I28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="K30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="K31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="K32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K34" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="7">
-        <v>42</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K35" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="K36" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="K37" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
       <c r="K38" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="K39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K39" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B40" s="1" t="s">
+      <c r="K40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K40" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="K41" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K42" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="A14:A38"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="D11:D12"/>
+  <mergeCells count="39">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="J29:J31"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="J26:J27"/>
     <mergeCell ref="J14:J16"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="H25:H27"/>
-    <mergeCell ref="J4:J7"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="J18:J19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="J4:J7"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="A14:A37"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C4:C6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J25" r:id="rId1" xr:uid="{D95D4A5D-20F4-48EC-9D6B-0DFC3F40799C}"/>
@@ -1511,8 +1645,12 @@
     <hyperlink ref="J8" r:id="rId13" xr:uid="{DE38EA62-1EC5-44CC-A013-93901FE4C0B0}"/>
     <hyperlink ref="J24" r:id="rId14" xr:uid="{21D85DDB-EB42-4E96-A4B5-7C3C922C94BC}"/>
     <hyperlink ref="J9" r:id="rId15" xr:uid="{E3499001-E08F-47CC-BA61-1975FA6B95F3}"/>
+    <hyperlink ref="J32" r:id="rId16" xr:uid="{2B15D5C1-094C-49CA-A380-F86AA73DEAC4}"/>
+    <hyperlink ref="J33" r:id="rId17" xr:uid="{A3284BC0-AE0A-4510-BD12-FC7ED627F37D}"/>
+    <hyperlink ref="J28" r:id="rId18" xr:uid="{9200CBC0-5446-4E6C-8538-B2188DCEC6EA}"/>
+    <hyperlink ref="J29" r:id="rId19" xr:uid="{779B5931-D582-4C3B-8642-0C15D647A1DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>